<commit_message>
Added Classes and OOP and Exceptions and Tools to list of readings for Programming for Data Science
Going to read about Exceptions and Tools
</commit_message>
<xml_diff>
--- a/UVA/1--Programming_For_Data_Science/Readings--for_Programming_for_Data_Science.xlsx
+++ b/UVA/1--Programming_For_Data_Science/Readings--for_Programming_for_Data_Science.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tlever/Tom_Levers_Git_Repository/UVA/1--Programming_For_Data_Science/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57FC7B0B-7A3B-6D4A-9EF8-96F698279B4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2AB35B4-1487-7E44-9B3E-A088235DC961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6480" yWindow="9780" windowWidth="28040" windowHeight="10840" xr2:uid="{6258D5FD-F2FA-BD40-BC8E-D382716EA801}"/>
+    <workbookView xWindow="4620" yWindow="8000" windowWidth="28040" windowHeight="10840" xr2:uid="{6258D5FD-F2FA-BD40-BC8E-D382716EA801}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Readings for Programming for Data Science</t>
   </si>
@@ -87,6 +87,12 @@
   </si>
   <si>
     <t>Updated: 09/27/22 by Tom Lever</t>
+  </si>
+  <si>
+    <t>Lutz 2019, Part VI, Classes and OOP</t>
+  </si>
+  <si>
+    <t>Lutz, 2019, Part VII: Exceptions and Tools</t>
   </si>
 </sst>
 </file>
@@ -470,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CE7F583-15FA-F847-A889-39CB314A797E}">
-  <dimension ref="A1:A21"/>
+  <dimension ref="A1:A23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -571,6 +577,16 @@
         <v>16</v>
       </c>
     </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>